<commit_message>
new image and report work.
</commit_message>
<xml_diff>
--- a/Domination/honours-project-report/images/Graphs.xlsx
+++ b/Domination/honours-project-report/images/Graphs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="30">
   <si>
     <t>Free</t>
   </si>
@@ -107,15 +107,26 @@
   <si>
     <t>A.I. Weight 4 Loser</t>
   </si>
+  <si>
+    <t>Loser Prediction Accuracy Over Game Length</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,8 +152,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -186,7 +200,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Accuracy </a:t>
+              <a:t> Accuracy Over Game Completion </a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -348,11 +362,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="113511424"/>
-        <c:axId val="113529984"/>
+        <c:axId val="117211520"/>
+        <c:axId val="117213440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="113511424"/>
+        <c:axId val="117211520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -386,7 +400,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113529984"/>
+        <c:crossAx val="117213440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -394,7 +408,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113529984"/>
+        <c:axId val="117213440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -429,16 +443,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113511424"/>
+        <c:crossAx val="117211520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -480,7 +495,13 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Prediction Accuracy</a:t>
+              <a:t> Prediction Accuracy </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Over Game Completion </a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -642,11 +663,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="113570176"/>
-        <c:axId val="113572096"/>
+        <c:axId val="117467776"/>
+        <c:axId val="117474048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="113570176"/>
+        <c:axId val="117467776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -680,7 +701,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113572096"/>
+        <c:crossAx val="117474048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -688,7 +709,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113572096"/>
+        <c:axId val="117474048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -723,16 +744,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113570176"/>
+        <c:crossAx val="117467776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -774,7 +796,13 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Prediction Accuracy</a:t>
+              <a:t> Prediction Accuracy </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Over Game Completion </a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -957,11 +985,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="113669632"/>
-        <c:axId val="113671552"/>
+        <c:axId val="117630080"/>
+        <c:axId val="117632000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="113669632"/>
+        <c:axId val="117630080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -995,7 +1023,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113671552"/>
+        <c:crossAx val="117632000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1003,7 +1031,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113671552"/>
+        <c:axId val="117632000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1038,16 +1066,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113669632"/>
+        <c:crossAx val="117630080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1313,11 +1342,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="119995008"/>
-        <c:axId val="120334976"/>
+        <c:axId val="117939584"/>
+        <c:axId val="117949952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="119995008"/>
+        <c:axId val="117939584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1350,7 +1379,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120334976"/>
+        <c:crossAx val="117949952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1358,7 +1387,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="120334976"/>
+        <c:axId val="117949952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1393,16 +1422,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119995008"/>
+        <c:crossAx val="117939584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1622,11 +1652,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="74084736"/>
-        <c:axId val="50278784"/>
+        <c:axId val="117701632"/>
+        <c:axId val="117703808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74084736"/>
+        <c:axId val="117701632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1659,7 +1689,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50278784"/>
+        <c:crossAx val="117703808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1667,7 +1697,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50278784"/>
+        <c:axId val="117703808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1702,16 +1732,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74084736"/>
+        <c:crossAx val="117701632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1719,7 +1750,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1931,11 +1962,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="73953280"/>
-        <c:axId val="73954816"/>
+        <c:axId val="117749248"/>
+        <c:axId val="117751168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73953280"/>
+        <c:axId val="117749248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1968,7 +1999,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73954816"/>
+        <c:crossAx val="117751168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1976,7 +2007,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73954816"/>
+        <c:axId val="117751168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2011,16 +2042,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73953280"/>
+        <c:crossAx val="117749248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2037,16 +2069,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>228599</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>219074</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2073,15 +2105,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>80961</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:colOff>23811</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>52386</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>142874</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2107,16 +2139,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>161926</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2142,16 +2174,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2177,16 +2209,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>585787</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171452</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2212,16 +2244,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2532,8 +2564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J20"/>
   <sheetViews>
-    <sheetView topLeftCell="L11" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2837,7 +2869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3122,8 +3154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView topLeftCell="J4" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3406,7 +3438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView topLeftCell="F10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3692,8 +3724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="G10" workbookViewId="0">
-      <selection sqref="A1:K22"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="AA24" sqref="AA24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4001,10 +4033,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4012,7 +4044,7 @@
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>16</v>
       </c>
@@ -4029,7 +4061,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -4064,7 +4096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3">
         <f>B2/(B2+C2)</f>
         <v>0.44</v>
@@ -4074,7 +4106,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -4109,13 +4141,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>B5/(B5+C5)</f>
         <v>0.78823529411764703</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="U7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -4150,7 +4187,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9">
         <f>B8/(B8+C8)</f>
         <v>0.34285714285714286</v>
@@ -4172,7 +4209,7 @@
         <v>0.29230769230769232</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -4207,7 +4244,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>B12/(B12+C12)</f>
         <v>0.22</v>
@@ -4303,6 +4340,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>